<commit_message>
preparing to fix temporal shift resolution limiting the duration filtering of vertical offsets.
</commit_message>
<xml_diff>
--- a/generated_files/time_shift_percentage_per_station_per_year.xlsx
+++ b/generated_files/time_shift_percentage_per_station_per_year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\cbi_data_quality\programs\noaa_lighthouse_problem\generated_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D83DADA-A850-4338-A6E5-AADBAC3A2396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6367D0A8-444D-44AA-BB3B-EFB486CCBD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -223,38 +223,35 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,56 +561,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="20"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -638,18 +635,18 @@
       <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -676,18 +673,18 @@
       <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="10">
         <v>0.22770000000000001</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -715,18 +712,18 @@
       <c r="H5" s="4">
         <v>0</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="10">
         <v>0.27060000000000001</v>
       </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -754,18 +751,18 @@
       <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="10">
         <v>0.52629999999999999</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -793,18 +790,18 @@
       <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="10">
         <v>0.34250000000000003</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -832,18 +829,18 @@
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="10">
         <v>8.77E-2</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -871,18 +868,18 @@
       <c r="H9" s="4">
         <v>0</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="10">
         <v>1.6335999999999999</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -910,18 +907,18 @@
       <c r="H10" s="4">
         <v>0</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="10">
         <v>0.99319999999999997</v>
       </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -949,18 +946,18 @@
       <c r="H11" s="4">
         <v>0</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="10">
         <v>0.14499999999999999</v>
       </c>
-      <c r="J11" s="18"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -988,18 +985,18 @@
       <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="10">
         <v>7.6300000000000007E-2</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
@@ -1027,18 +1024,18 @@
       <c r="H13" s="4">
         <v>0</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="10">
         <v>0.28539999999999999</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
@@ -1066,18 +1063,18 @@
       <c r="H14" s="4">
         <v>0</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="10">
         <v>2.1884000000000001</v>
       </c>
-      <c r="J14" s="18"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
@@ -1105,18 +1102,18 @@
       <c r="H15" s="8">
         <v>39.695700000000002</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="10">
         <v>1.5639000000000001</v>
       </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
@@ -1144,18 +1141,18 @@
       <c r="H16" s="5">
         <v>96.803200000000004</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="10">
         <v>0.9153</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
@@ -1183,18 +1180,18 @@
       <c r="H17" s="5">
         <v>97.132400000000004</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="10">
         <v>2.4908999999999999</v>
       </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2">

</xml_diff>